<commit_message>
Correção de caso de teste
</commit_message>
<xml_diff>
--- a/docs/Casos de Teste.xlsx
+++ b/docs/Casos de Teste.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162912"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Entrada</t>
   </si>
@@ -125,13 +125,16 @@
   </si>
   <si>
     <t>Senha com 8 caracteres iguais sendo 4 maiúsculos e 4 minúsculos. VVVVvvvv</t>
+  </si>
+  <si>
+    <t>Pontuação: 1; Força = "Easy"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -510,18 +513,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -532,7 +535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -543,7 +546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="34.5" customHeight="1">
+    <row r="3" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -554,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="36" customHeight="1">
+    <row r="4" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -565,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="39.75" customHeight="1">
+    <row r="5" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -576,7 +579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45">
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -587,7 +590,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="51.75" customHeight="1">
+    <row r="7" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -598,7 +601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="48.75" customHeight="1">
+    <row r="8" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -609,7 +612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="49.5" customHeight="1">
+    <row r="9" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -620,7 +623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="50.25" customHeight="1">
+    <row r="10" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -631,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="37.5" customHeight="1">
+    <row r="11" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -642,7 +645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -653,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -664,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -675,7 +678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="50.25" customHeight="1">
+    <row r="15" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -686,18 +689,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="45">
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="78" customHeight="1">
+    <row r="17" spans="1:3" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -708,7 +711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="45">
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -719,7 +722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="45">
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -730,7 +733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
@@ -741,7 +744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" customHeight="1">
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -752,7 +755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="45">
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>36</v>
       </c>

</xml_diff>